<commit_message>
Added 2 x Molex Micro-fits for Remote Modules
Potential, use is not confirmed yet
</commit_message>
<xml_diff>
--- a/connectors/ts_standard_connectors.xlsx
+++ b/connectors/ts_standard_connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwjde\Documents\GitHub\TS_24_Components\connectors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\connectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAFB249-DC36-4C63-A84C-955DAFBDEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315D8CCC-5B32-4FF0-B38F-27982FF1BE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1545" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="197">
   <si>
     <t>Part Number</t>
   </si>
@@ -625,6 +625,18 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/en/products/detail/amphenol-sine-systems-corp/ATF13-08PA-BM13/10322694</t>
+  </si>
+  <si>
+    <t>WM7490-ND</t>
+  </si>
+  <si>
+    <t>2266-430451801-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/wec/430451801/18847960</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/molex/0430451601/3044582</t>
   </si>
 </sst>
 </file>
@@ -963,15 +975,15 @@
       <selection activeCell="J7" sqref="A1:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -982,28 +994,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFC7277-B90C-4D40-A394-1A49AC3F5C48}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="102.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="102.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1167,7 +1179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1208,7 +1220,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1249,7 +1261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1331,7 +1343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1372,7 +1384,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1413,7 +1425,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1454,7 +1466,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -1519,19 +1531,19 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" customWidth="1"/>
-    <col min="10" max="10" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1601,7 +1613,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -1636,7 +1648,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>126</v>
       </c>
@@ -1671,7 +1683,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -1706,7 +1718,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -1741,7 +1753,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -1776,7 +1788,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -1811,7 +1823,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -1846,7 +1858,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -1881,7 +1893,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -1916,7 +1928,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -1951,7 +1963,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -1986,7 +1998,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -2056,7 +2068,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -2126,7 +2138,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>146</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -2196,7 +2208,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -2231,7 +2243,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>152</v>
       </c>
@@ -2266,7 +2278,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>154</v>
       </c>
@@ -2301,7 +2313,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>156</v>
       </c>
@@ -2336,7 +2348,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>158</v>
       </c>
@@ -2371,7 +2383,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>159</v>
       </c>
@@ -2406,7 +2418,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -2441,7 +2453,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>161</v>
       </c>
@@ -2476,7 +2488,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>176</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -2559,25 +2571,25 @@
       <selection activeCell="J8" sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6328125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2619,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>179</v>
       </c>
@@ -2649,19 +2661,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2690,7 +2702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -2719,7 +2731,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>185</v>
       </c>
@@ -2748,7 +2760,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>184</v>
       </c>
@@ -2777,7 +2789,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>186</v>
       </c>
@@ -2820,21 +2832,21 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="16.54296875" customWidth="1"/>
-    <col min="11" max="11" width="19.7265625" customWidth="1"/>
-    <col min="12" max="12" width="15.90625" customWidth="1"/>
-    <col min="13" max="13" width="42.1796875" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2875,7 +2887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -2917,22 +2929,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB4216D-9057-4A38-8D25-BDA25A2F9C93}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2973,7 +2985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39300020</v>
       </c>
@@ -3012,7 +3024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>39300040</v>
       </c>
@@ -3051,7 +3063,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>39300060</v>
       </c>
@@ -3090,7 +3102,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>39300080</v>
       </c>
@@ -3129,7 +3141,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>39300100</v>
       </c>
@@ -3168,7 +3180,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>39300120</v>
       </c>
@@ -3207,7 +3219,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>39300140</v>
       </c>
@@ -3246,7 +3258,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>39300160</v>
       </c>
@@ -3285,7 +3297,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>39300180</v>
       </c>
@@ -3324,7 +3336,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>39300200</v>
       </c>
@@ -3363,7 +3375,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>39300220</v>
       </c>
@@ -3402,7 +3414,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>39300240</v>
       </c>
@@ -3441,7 +3453,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>39293026</v>
       </c>
@@ -3480,7 +3492,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>39293046</v>
       </c>
@@ -3519,7 +3531,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>39293066</v>
       </c>
@@ -3558,7 +3570,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>39293086</v>
       </c>
@@ -3597,7 +3609,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>39293106</v>
       </c>
@@ -3636,7 +3648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>39293126</v>
       </c>
@@ -3675,7 +3687,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>39293146</v>
       </c>
@@ -3714,7 +3726,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>39293166</v>
       </c>
@@ -3753,7 +3765,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>39293206</v>
       </c>
@@ -3792,7 +3804,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>436500500</v>
       </c>
@@ -3835,7 +3847,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>436500600</v>
       </c>
@@ -3878,7 +3890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>436500700</v>
       </c>
@@ -3921,7 +3933,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>39288100</v>
       </c>
@@ -3958,6 +3970,89 @@
       </c>
       <c r="L26" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>430451601</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27">
+        <v>90</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27">
+        <f>A27</f>
+        <v>430451601</v>
+      </c>
+      <c r="I27" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27">
+        <v>430451601</v>
+      </c>
+      <c r="K27" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" t="s">
+        <v>193</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>430451801</v>
+      </c>
+      <c r="B28">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28">
+        <v>430451801</v>
+      </c>
+      <c r="I28" t="s">
+        <v>80</v>
+      </c>
+      <c r="J28">
+        <v>430451801</v>
+      </c>
+      <c r="K28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" t="s">
+        <v>194</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -3965,6 +4060,8 @@
     <hyperlink ref="M24" r:id="rId1" xr:uid="{B56F008D-7E6D-41AE-A693-3CFFF3BBD5F7}"/>
     <hyperlink ref="M23" r:id="rId2" xr:uid="{1583D851-1A0F-467C-97DC-F42A8FED5404}"/>
     <hyperlink ref="M25" r:id="rId3" xr:uid="{F38D1959-4FBD-40D2-A83D-03508E7963E3}"/>
+    <hyperlink ref="M28" r:id="rId4" xr:uid="{4A016966-2569-41C8-98EE-174801ECF565}"/>
+    <hyperlink ref="M27" r:id="rId5" xr:uid="{E6062D2F-D4DB-495E-8EA1-16A2E05AAC15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3978,14 +4075,14 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="18.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" customWidth="1"/>
-    <col min="11" max="11" width="12.90625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4026,7 +4123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4083,15 +4180,15 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4132,7 +4229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4183,12 +4280,12 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4229,7 +4326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -4270,7 +4367,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>3</v>
       </c>
@@ -4299,7 +4396,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>4</v>
       </c>
@@ -4328,7 +4425,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>5</v>
       </c>
@@ -4357,7 +4454,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>6</v>
       </c>
@@ -4386,7 +4483,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>7</v>
       </c>
@@ -4415,7 +4512,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>8</v>
       </c>
@@ -4444,7 +4541,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>9</v>
       </c>
@@ -4473,7 +4570,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>10</v>
       </c>
@@ -4502,7 +4599,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -4559,16 +4656,16 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" customWidth="1"/>
-    <col min="6" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="27.54296875" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4597,7 +4694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
Added 20 pin micro-fit th r/a header
</commit_message>
<xml_diff>
--- a/connectors/ts_standard_connectors.xlsx
+++ b/connectors/ts_standard_connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\connectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315D8CCC-5B32-4FF0-B38F-27982FF1BE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D0BA4A-5AE5-4A31-8F94-FAB5C164A642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="199">
   <si>
     <t>Part Number</t>
   </si>
@@ -637,6 +637,12 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/en/products/detail/molex/0430451601/3044582</t>
+  </si>
+  <si>
+    <t>WM7492-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/en/products/detail/molex/0430452001/3044584</t>
   </si>
 </sst>
 </file>
@@ -2929,10 +2935,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB4216D-9057-4A38-8D25-BDA25A2F9C93}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,6 +4061,47 @@
         <v>195</v>
       </c>
     </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>430452001</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29">
+        <v>90</v>
+      </c>
+      <c r="F29" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29">
+        <v>430452001</v>
+      </c>
+      <c r="I29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J29">
+        <v>430452001</v>
+      </c>
+      <c r="K29" t="s">
+        <v>81</v>
+      </c>
+      <c r="L29" t="s">
+        <v>197</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M24" r:id="rId1" xr:uid="{B56F008D-7E6D-41AE-A693-3CFFF3BBD5F7}"/>
@@ -4062,6 +4109,7 @@
     <hyperlink ref="M25" r:id="rId3" xr:uid="{F38D1959-4FBD-40D2-A83D-03508E7963E3}"/>
     <hyperlink ref="M28" r:id="rId4" xr:uid="{4A016966-2569-41C8-98EE-174801ECF565}"/>
     <hyperlink ref="M27" r:id="rId5" xr:uid="{E6062D2F-D4DB-495E-8EA1-16A2E05AAC15}"/>
+    <hyperlink ref="M29" r:id="rId6" xr:uid="{3C7FB8A9-CF68-44AA-A5F5-1474AF1E61C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 8 pin molex microfit header
</commit_message>
<xml_diff>
--- a/connectors/ts_standard_connectors.xlsx
+++ b/connectors/ts_standard_connectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\TS_24_Components\connectors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D0BA4A-5AE5-4A31-8F94-FAB5C164A642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221CCF21-9381-4BC6-914A-F9576C56C9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="105" windowWidth="86355" windowHeight="15495" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="201">
   <si>
     <t>Part Number</t>
   </si>
@@ -643,6 +643,12 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/en/products/detail/molex/0430452001/3044584</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0430450815/3044333</t>
+  </si>
+  <si>
+    <t>WM7067DKR-ND</t>
   </si>
 </sst>
 </file>
@@ -2935,10 +2941,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB4216D-9057-4A38-8D25-BDA25A2F9C93}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4102,6 +4108,47 @@
         <v>198</v>
       </c>
     </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>430450815</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30">
+        <v>90</v>
+      </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30">
+        <v>430450815</v>
+      </c>
+      <c r="I30" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30">
+        <v>430450815</v>
+      </c>
+      <c r="K30" t="s">
+        <v>81</v>
+      </c>
+      <c r="L30" t="s">
+        <v>200</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M24" r:id="rId1" xr:uid="{B56F008D-7E6D-41AE-A693-3CFFF3BBD5F7}"/>
@@ -4110,6 +4157,7 @@
     <hyperlink ref="M28" r:id="rId4" xr:uid="{4A016966-2569-41C8-98EE-174801ECF565}"/>
     <hyperlink ref="M27" r:id="rId5" xr:uid="{E6062D2F-D4DB-495E-8EA1-16A2E05AAC15}"/>
     <hyperlink ref="M29" r:id="rId6" xr:uid="{3C7FB8A9-CF68-44AA-A5F5-1474AF1E61C6}"/>
+    <hyperlink ref="M30" r:id="rId7" xr:uid="{15B07E7E-BF0F-4978-852C-C3E56B9DD554}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>